<commit_message>
Correction Planning et visu Appel Micro
Correction du planning et création du visuel pour l'appel Micro. Après
test avec les données clients, on retombe bien sur les mêmes valeurs.
</commit_message>
<xml_diff>
--- a/bin/export/HoraireCompetition.xlsx
+++ b/bin/export/HoraireCompetition.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Id Epreuve</t>
   </si>
@@ -38,21 +38,6 @@
     <t xml:space="preserve"> Battement Epreuve</t>
   </si>
   <si>
-    <t>Statique</t>
-  </si>
-  <si>
-    <t>DWF</t>
-  </si>
-  <si>
-    <t>Speed 100</t>
-  </si>
-  <si>
-    <t>DNF</t>
-  </si>
-  <si>
-    <t>16*50</t>
-  </si>
-  <si>
     <t>Déroulement des EPREUVE</t>
   </si>
   <si>
@@ -66,6 +51,18 @@
   </si>
   <si>
     <t>Battement</t>
+  </si>
+  <si>
+    <t>sta</t>
+  </si>
+  <si>
+    <t>dwf</t>
+  </si>
+  <si>
+    <t>spd</t>
+  </si>
+  <si>
+    <t>dnf</t>
   </si>
 </sst>
 </file>
@@ -377,33 +374,52 @@
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -413,25 +429,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,7 +736,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +766,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>0.42708333333333331</v>
@@ -781,7 +778,7 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -792,7 +789,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -801,18 +798,18 @@
         <v>3</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>9</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -821,7 +818,7 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>5</v>
@@ -832,7 +829,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -841,18 +838,18 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>9</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
+      <c r="A6">
+        <v>1650</v>
       </c>
       <c r="C6">
         <v>30</v>
@@ -861,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -880,254 +877,254 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="16" t="str">
+      <c r="A1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="8" t="str">
         <f>Données!A2</f>
-        <v>Statique</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4">
+        <v>sta</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="2">
         <f>E2-TIME(0,Données!D2,0)-TIME(0,Données!C2,0)</f>
         <v>0.40416666666666667</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7">
+      <c r="A2" s="18"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="3">
         <f>Données!B2</f>
         <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8">
+      <c r="A3" s="18"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="4">
         <f>E2+TIME(0,(Données!E2*Données!F2),0)</f>
-        <v>0.44444444444444442</v>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11">
+      <c r="A4" s="18"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="5">
         <f>TIME(0,Données!G2,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="16" t="str">
-        <f>Données!A2</f>
-        <v>Statique</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="12">
+      <c r="A5" s="18"/>
+      <c r="B5" s="8" t="str">
+        <f>Données!A3</f>
+        <v>dwf</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="6">
         <f>E6-TIME(0,Données!D3,0)-TIME(0,Données!C3,0)</f>
-        <v>0.4284722222222222</v>
+        <v>0.45277777777777778</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="8">
+      <c r="A6" s="18"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="4">
         <f>E3+E4</f>
-        <v>0.45138888888888884</v>
+        <v>0.47569444444444442</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="8">
+      <c r="A7" s="18"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="4">
         <f>E6+TIME(0,(Données!E3*Données!F3),0)</f>
-        <v>0.48263888888888884</v>
+        <v>0.53194444444444444</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11">
+      <c r="A8" s="18"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="5">
         <f>TIME(0,Données!G3,0)</f>
-        <v>6.9444444444444441E-3</v>
+        <v>2.7083333333333334E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="16" t="str">
-        <f>Données!A3</f>
-        <v>DWF</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4">
+      <c r="A9" s="18"/>
+      <c r="B9" s="8" t="str">
+        <f>Données!A4</f>
+        <v>spd</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="2">
         <f>E10-TIME(0,Données!D4,0)-TIME(0,Données!C4,0)</f>
-        <v>0.46666666666666662</v>
+        <v>0.53611111111111109</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="8">
+      <c r="A10" s="18"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="4">
         <f>E7+E8</f>
-        <v>0.48958333333333326</v>
+        <v>0.55902777777777779</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="8">
+      <c r="A11" s="18"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="4">
         <f>E10+TIME(0,(Données!E4*Données!F4),0)</f>
-        <v>0.50694444444444442</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11">
+      <c r="A12" s="18"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="5">
         <f>TIME(0,Données!G4,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="16" t="str">
-        <f>Données!A4</f>
-        <v>Speed 100</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="12">
+      <c r="A13" s="18"/>
+      <c r="B13" s="8" t="str">
+        <f>Données!A5</f>
+        <v>dnf</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="6">
         <f>E14-TIME(0,Données!D5,0)-TIME(0,Données!C5,0)</f>
-        <v>0.4909722222222222</v>
+        <v>0.56736111111111109</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="8">
+      <c r="A14" s="18"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="4">
         <f>E11+E12</f>
-        <v>0.51388888888888884</v>
+        <v>0.59027777777777779</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="8">
+      <c r="A15" s="18"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="4">
         <f>E14+TIME(0,(Données!E5*Données!F5),0)</f>
-        <v>0.54513888888888884</v>
+        <v>0.64652777777777781</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11">
+      <c r="A16" s="18"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="5">
         <f>TIME(0,Données!G5,0)</f>
-        <v>6.9444444444444441E-3</v>
+        <v>6.2499999999999995E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="13" t="str">
-        <f>Données!A5</f>
-        <v>DNF</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="12">
+      <c r="A17" s="18"/>
+      <c r="B17" s="20">
+        <f>Données!A6</f>
+        <v>1650</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="6">
         <f>E18-TIME(0,Données!D6,0)-TIME(0,Données!C6,0)</f>
-        <v>0.52916666666666656</v>
+        <v>0.62986111111111109</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="8">
+      <c r="A18" s="18"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="4">
         <f>E15+E16</f>
-        <v>0.55208333333333326</v>
+        <v>0.65277777777777779</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="22">
+      <c r="A19" s="19"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="7">
         <f>E18+TIME(0,(Données!E6*Données!F6),0)</f>
-        <v>0.5659722222222221</v>
+        <v>0.71666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -1148,15 +1145,15 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout Fiche de prise de Perf
Ajout des fiches de prise de performance dans le fichier
"PlanningEpreuve".
</commit_message>
<xml_diff>
--- a/bin/export/HoraireCompetition.xlsx
+++ b/bin/export/HoraireCompetition.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Données" sheetId="1" r:id="rId1"/>
@@ -384,6 +384,15 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,15 +419,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -733,13 +733,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -874,254 +879,255 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil2"/>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="str">
+      <c r="B1" s="11" t="str">
         <f>Données!A2</f>
         <v>sta</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="12"/>
+      <c r="D1" s="15"/>
       <c r="E1" s="2">
         <f>E2-TIME(0,Données!D2,0)-TIME(0,Données!C2,0)</f>
         <v>0.40416666666666667</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="13" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="3">
         <f>Données!B2</f>
         <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="4">
         <f>E2+TIME(0,(Données!E2*Données!F2),0)</f>
         <v>0.46875</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="19"/>
       <c r="E4" s="5">
         <f>TIME(0,Données!G2,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="8" t="str">
+      <c r="A5" s="9"/>
+      <c r="B5" s="11" t="str">
         <f>Données!A3</f>
         <v>dwf</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="6">
         <f>E6-TIME(0,Données!D3,0)-TIME(0,Données!C3,0)</f>
         <v>0.45277777777777778</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="13" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="4">
         <f>E3+E4</f>
         <v>0.47569444444444442</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="4">
         <f>E6+TIME(0,(Données!E3*Données!F3),0)</f>
         <v>0.53194444444444444</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="15" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="5">
         <f>TIME(0,Données!G3,0)</f>
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="8" t="str">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11" t="str">
         <f>Données!A4</f>
         <v>spd</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="2">
         <f>E10-TIME(0,Données!D4,0)-TIME(0,Données!C4,0)</f>
         <v>0.53611111111111109</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="13" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="4">
         <f>E7+E8</f>
         <v>0.55902777777777779</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="13" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="4">
         <f>E10+TIME(0,(Données!E4*Données!F4),0)</f>
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="15" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="5">
         <f>TIME(0,Données!G4,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="8" t="str">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11" t="str">
         <f>Données!A5</f>
         <v>dnf</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="6">
         <f>E14-TIME(0,Données!D5,0)-TIME(0,Données!C5,0)</f>
         <v>0.56736111111111109</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="13" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="4">
         <f>E11+E12</f>
         <v>0.59027777777777779</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="13" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="4">
         <f>E14+TIME(0,(Données!E5*Données!F5),0)</f>
         <v>0.64652777777777781</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="15" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="5">
         <f>TIME(0,Données!G5,0)</f>
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="20">
         <f>Données!A6</f>
         <v>1650</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="6">
         <f>E18-TIME(0,Données!D6,0)-TIME(0,Données!C6,0)</f>
         <v>0.62986111111111109</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="21"/>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="4">
         <f>E15+E16</f>
         <v>0.65277777777777779</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="22"/>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="7">
         <f>E18+TIME(0,(Données!E6*Données!F6),0)</f>
         <v>0.71666666666666667</v>
@@ -1129,6 +1135,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
     <mergeCell ref="A1:A19"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:D13"/>
@@ -1145,15 +1160,6 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Encodage et verif fonction modify
</commit_message>
<xml_diff>
--- a/bin/export/HoraireCompetition.xlsx
+++ b/bin/export/HoraireCompetition.xlsx
@@ -39,6 +39,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -341,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="20" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -353,15 +356,6 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -389,6 +383,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -398,6 +401,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,11 +861,12 @@
   <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="11.42578125" style="22"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -871,7 +876,7 @@
         <f>[1]PlanningCompetition!A1</f>
         <v>Id Epreuve</v>
       </c>
-      <c r="B1" t="str">
+      <c r="B1" s="22" t="str">
         <f>[1]PlanningCompetition!B1</f>
         <v xml:space="preserve"> HeureOuverture(1ereEpreuve)</v>
       </c>
@@ -969,7 +974,7 @@
         <f>[1]PlanningCompetition!A2</f>
         <v>sta</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="22">
         <f>[1]PlanningCompetition!B2</f>
         <v>0.42708333333333331</v>
       </c>
@@ -1067,7 +1072,7 @@
         <f>[1]PlanningCompetition!A3</f>
         <v>dwf</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="22">
         <f>[1]PlanningCompetition!B3</f>
         <v>0</v>
       </c>
@@ -1165,7 +1170,7 @@
         <f>[1]PlanningCompetition!A4</f>
         <v>spd</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="22">
         <f>[1]PlanningCompetition!B4</f>
         <v>0</v>
       </c>
@@ -1263,7 +1268,7 @@
         <f>[1]PlanningCompetition!A5</f>
         <v>dnf</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="22">
         <f>[1]PlanningCompetition!B5</f>
         <v>0</v>
       </c>
@@ -1361,7 +1366,7 @@
         <f>[1]PlanningCompetition!A6</f>
         <v>1650</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="22">
         <f>[1]PlanningCompetition!B6</f>
         <v>0</v>
       </c>
@@ -1459,7 +1464,7 @@
         <f>[1]PlanningCompetition!A7</f>
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="22">
         <f>[1]PlanningCompetition!B7</f>
         <v>0</v>
       </c>
@@ -1557,7 +1562,7 @@
         <f>[1]PlanningCompetition!A8</f>
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="22">
         <f>[1]PlanningCompetition!B8</f>
         <v>0</v>
       </c>
@@ -1655,7 +1660,7 @@
         <f>[1]PlanningCompetition!A9</f>
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="22">
         <f>[1]PlanningCompetition!B9</f>
         <v>0</v>
       </c>
@@ -1753,7 +1758,7 @@
         <f>[1]PlanningCompetition!A10</f>
         <v>0</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="22">
         <f>[1]PlanningCompetition!B10</f>
         <v>0</v>
       </c>
@@ -1851,7 +1856,7 @@
         <f>[1]PlanningCompetition!A11</f>
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="22">
         <f>[1]PlanningCompetition!B11</f>
         <v>0</v>
       </c>
@@ -1949,7 +1954,7 @@
         <f>[1]PlanningCompetition!A12</f>
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="22">
         <f>[1]PlanningCompetition!B12</f>
         <v>0</v>
       </c>
@@ -2047,7 +2052,7 @@
         <f>[1]PlanningCompetition!A13</f>
         <v>0</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="22">
         <f>[1]PlanningCompetition!B13</f>
         <v>0</v>
       </c>
@@ -2145,7 +2150,7 @@
         <f>[1]PlanningCompetition!A14</f>
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="22">
         <f>[1]PlanningCompetition!B14</f>
         <v>0</v>
       </c>
@@ -2243,7 +2248,7 @@
         <f>[1]PlanningCompetition!A15</f>
         <v>0</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="22">
         <f>[1]PlanningCompetition!B15</f>
         <v>0</v>
       </c>
@@ -2341,7 +2346,7 @@
         <f>[1]PlanningCompetition!A16</f>
         <v>0</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="22">
         <f>[1]PlanningCompetition!B16</f>
         <v>0</v>
       </c>
@@ -2439,7 +2444,7 @@
         <f>[1]PlanningCompetition!A17</f>
         <v>0</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="22">
         <f>[1]PlanningCompetition!B17</f>
         <v>0</v>
       </c>
@@ -2537,7 +2542,7 @@
         <f>[1]PlanningCompetition!A18</f>
         <v>0</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="22">
         <f>[1]PlanningCompetition!B18</f>
         <v>0</v>
       </c>
@@ -2635,7 +2640,7 @@
         <f>[1]PlanningCompetition!A19</f>
         <v>0</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="22">
         <f>[1]PlanningCompetition!B19</f>
         <v>0</v>
       </c>
@@ -2733,7 +2738,7 @@
         <f>[1]PlanningCompetition!A20</f>
         <v>0</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="22">
         <f>[1]PlanningCompetition!B20</f>
         <v>0</v>
       </c>
@@ -2831,7 +2836,7 @@
         <f>[1]PlanningCompetition!A21</f>
         <v>0</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="22">
         <f>[1]PlanningCompetition!B21</f>
         <v>0</v>
       </c>
@@ -2929,7 +2934,7 @@
         <f>[1]PlanningCompetition!A22</f>
         <v>0</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="22">
         <f>[1]PlanningCompetition!B22</f>
         <v>0</v>
       </c>
@@ -3027,7 +3032,7 @@
         <f>[1]PlanningCompetition!A23</f>
         <v>0</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="22">
         <f>[1]PlanningCompetition!B23</f>
         <v>0</v>
       </c>
@@ -3125,7 +3130,7 @@
         <f>[1]PlanningCompetition!A24</f>
         <v>0</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="22">
         <f>[1]PlanningCompetition!B24</f>
         <v>0</v>
       </c>
@@ -3223,7 +3228,7 @@
         <f>[1]PlanningCompetition!A25</f>
         <v>0</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="22">
         <f>[1]PlanningCompetition!B25</f>
         <v>0</v>
       </c>
@@ -3321,7 +3326,7 @@
         <f>[1]PlanningCompetition!A26</f>
         <v>0</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="22">
         <f>[1]PlanningCompetition!B26</f>
         <v>0</v>
       </c>
@@ -3419,7 +3424,7 @@
         <f>[1]PlanningCompetition!A27</f>
         <v>0</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="22">
         <f>[1]PlanningCompetition!B27</f>
         <v>0</v>
       </c>
@@ -3517,7 +3522,7 @@
         <f>[1]PlanningCompetition!A28</f>
         <v>0</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="22">
         <f>[1]PlanningCompetition!B28</f>
         <v>0</v>
       </c>
@@ -3615,7 +3620,7 @@
         <f>[1]PlanningCompetition!A29</f>
         <v>0</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="22">
         <f>[1]PlanningCompetition!B29</f>
         <v>0</v>
       </c>
@@ -3713,7 +3718,7 @@
         <f>[1]PlanningCompetition!A30</f>
         <v>0</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="22">
         <f>[1]PlanningCompetition!B30</f>
         <v>0</v>
       </c>
@@ -3811,7 +3816,7 @@
         <f>[1]PlanningCompetition!A31</f>
         <v>0</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="22">
         <f>[1]PlanningCompetition!B31</f>
         <v>0</v>
       </c>
@@ -3909,7 +3914,7 @@
         <f>[1]PlanningCompetition!A32</f>
         <v>0</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="22">
         <f>[1]PlanningCompetition!B32</f>
         <v>0</v>
       </c>
@@ -4007,7 +4012,7 @@
         <f>[1]PlanningCompetition!A33</f>
         <v>0</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="22">
         <f>[1]PlanningCompetition!B33</f>
         <v>0</v>
       </c>
@@ -4105,7 +4110,7 @@
         <f>[1]PlanningCompetition!A34</f>
         <v>0</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="22">
         <f>[1]PlanningCompetition!B34</f>
         <v>0</v>
       </c>
@@ -4203,7 +4208,7 @@
         <f>[1]PlanningCompetition!A35</f>
         <v>0</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="22">
         <f>[1]PlanningCompetition!B35</f>
         <v>0</v>
       </c>
@@ -4301,7 +4306,7 @@
         <f>[1]PlanningCompetition!A36</f>
         <v>0</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="22">
         <f>[1]PlanningCompetition!B36</f>
         <v>0</v>
       </c>
@@ -4399,7 +4404,7 @@
         <f>[1]PlanningCompetition!A37</f>
         <v>0</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="22">
         <f>[1]PlanningCompetition!B37</f>
         <v>0</v>
       </c>
@@ -4497,7 +4502,7 @@
         <f>[1]PlanningCompetition!A38</f>
         <v>0</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="22">
         <f>[1]PlanningCompetition!B38</f>
         <v>0</v>
       </c>
@@ -4595,7 +4600,7 @@
         <f>[1]PlanningCompetition!A39</f>
         <v>0</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="22">
         <f>[1]PlanningCompetition!B39</f>
         <v>0</v>
       </c>
@@ -4693,7 +4698,7 @@
         <f>[1]PlanningCompetition!A40</f>
         <v>0</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="22">
         <f>[1]PlanningCompetition!B40</f>
         <v>0</v>
       </c>
@@ -4810,245 +4815,245 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="10" t="str">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="str">
         <f>Données!A2</f>
         <v>sta</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="1">
         <f>E3-TIME(0,Données!D2,0)-TIME(0,Données!C2,0)</f>
         <v>0.40416666666666667</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="15" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="13"/>
       <c r="E3" s="2">
         <f>Données!B2</f>
         <v>0.42708333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="15" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="3">
         <f>E3+TIME(0,(Données!E2*Données!F2),0)</f>
         <v>0.4770833333333333</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="17" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="4">
         <f>TIME(0,Données!G2,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10" t="str">
+      <c r="A6" s="17"/>
+      <c r="B6" s="7" t="str">
         <f>Données!A3</f>
         <v>dwf</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="5">
         <f>E7-TIME(0,Données!D3,0)-TIME(0,Données!C3,0)</f>
         <v>0.46111111111111108</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="15" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="3">
         <f>E4+E5</f>
         <v>0.48402777777777772</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="15" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="16"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="3">
         <f>E7+TIME(0,(Données!E3*Données!F3),0)</f>
         <v>0.54027777777777775</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="17" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="4">
         <f>TIME(0,Données!G3,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="10" t="str">
+      <c r="A10" s="17"/>
+      <c r="B10" s="7" t="str">
         <f>Données!A4</f>
         <v>spd</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="1">
         <f>E11-TIME(0,Données!D4,0)-TIME(0,Données!C4,0)</f>
         <v>0.52430555555555547</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="15" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="3">
         <f>E8+E9</f>
         <v>0.54722222222222217</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="15" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="16"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="3">
         <f>E11+TIME(0,(Données!E4*Données!F4),0)</f>
         <v>0.57638888888888884</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="17" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="4">
         <f>TIME(0,Données!G4,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="10" t="str">
+      <c r="A14" s="17"/>
+      <c r="B14" s="7" t="str">
         <f>Données!A5</f>
         <v>dnf</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="14"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="5">
         <f>E15-TIME(0,Données!D5,0)-TIME(0,Données!C5,0)</f>
         <v>0.56041666666666656</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="15" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="3">
         <f>E12+E13</f>
         <v>0.58333333333333326</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="15" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="16"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="3">
         <f>E15+TIME(0,(Données!E5*Données!F5),0)</f>
         <v>0.63958333333333328</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="17" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="4">
         <f>TIME(0,Données!G5,0)</f>
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="19">
         <f>Données!A6</f>
         <v>1650</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="14"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="5">
         <f>E19-TIME(0,Données!D6,0)-TIME(0,Données!C6,0)</f>
         <v>0.62361111111111101</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="20"/>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="3">
         <f>E16+E17</f>
         <v>0.6465277777777777</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="21"/>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="18"/>
+      <c r="D20" s="15"/>
       <c r="E20" s="6">
         <f>E19+TIME(0,(Données!E6*Données!F6),0)</f>
         <v>0.71041666666666659</v>
@@ -5056,15 +5061,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="A2:A20"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C14:D14"/>
@@ -5081,6 +5077,15 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
OPEN APNEE LYON - POST-EVENT
</commit_message>
<xml_diff>
--- a/bin/export/HoraireCompetition.xlsx
+++ b/bin/export/HoraireCompetition.xlsx
@@ -481,7 +481,7 @@
             <v>4</v>
           </cell>
           <cell r="G2">
-            <v>10</v>
+            <v>17</v>
           </cell>
         </row>
         <row r="3">
@@ -501,7 +501,7 @@
             <v>9</v>
           </cell>
           <cell r="G3">
-            <v>25</v>
+            <v>29</v>
           </cell>
         </row>
         <row r="4">
@@ -541,7 +541,7 @@
             <v>9</v>
           </cell>
           <cell r="G5">
-            <v>10</v>
+            <v>14</v>
           </cell>
         </row>
         <row r="6">
@@ -996,7 +996,7 @@
       </c>
       <c r="G2">
         <f>[1]PlanningCompetition!G2</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H2">
         <f>[1]PlanningCompetition!H2</f>
@@ -1094,7 +1094,7 @@
       </c>
       <c r="G3">
         <f>[1]PlanningCompetition!G3</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H3">
         <f>[1]PlanningCompetition!H3</f>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="G5">
         <f>[1]PlanningCompetition!G5</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H5">
         <f>[1]PlanningCompetition!H5</f>
@@ -4808,7 +4808,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4867,7 +4867,7 @@
       <c r="D5" s="19"/>
       <c r="E5" s="4">
         <f>TIME(0,Données!G2,0)</f>
-        <v>6.9444444444444441E-3</v>
+        <v>1.1805555555555555E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4882,7 +4882,7 @@
       <c r="D6" s="15"/>
       <c r="E6" s="5">
         <f>E7-TIME(0,Données!D3,0)-TIME(0,Données!C3,0)</f>
-        <v>0.44444444444444442</v>
+        <v>0.44930555555555557</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4894,7 +4894,7 @@
       <c r="D7" s="17"/>
       <c r="E7" s="3">
         <f>E4+E5</f>
-        <v>0.46736111111111106</v>
+        <v>0.47222222222222221</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4906,7 +4906,7 @@
       <c r="D8" s="17"/>
       <c r="E8" s="3">
         <f>E7+TIME(0,(Données!E3*Données!F3),0)</f>
-        <v>0.52361111111111103</v>
+        <v>0.52847222222222223</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4918,7 +4918,7 @@
       <c r="D9" s="19"/>
       <c r="E9" s="4">
         <f>TIME(0,Données!G3,0)</f>
-        <v>1.7361111111111112E-2</v>
+        <v>2.013888888888889E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4933,7 +4933,7 @@
       <c r="D10" s="15"/>
       <c r="E10" s="1">
         <f>E11-TIME(0,Données!D4,0)-TIME(0,Données!C4,0)</f>
-        <v>0.51805555555555549</v>
+        <v>0.52569444444444446</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4945,7 +4945,7 @@
       <c r="D11" s="17"/>
       <c r="E11" s="3">
         <f>E8+E9</f>
-        <v>0.54097222222222219</v>
+        <v>0.54861111111111116</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4957,7 +4957,7 @@
       <c r="D12" s="17"/>
       <c r="E12" s="3">
         <f>E11+TIME(0,(Données!E4*Données!F4),0)</f>
-        <v>0.56527777777777777</v>
+        <v>0.57291666666666674</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4984,7 +4984,7 @@
       <c r="D14" s="15"/>
       <c r="E14" s="5">
         <f>E15-TIME(0,Données!D5,0)-TIME(0,Données!C5,0)</f>
-        <v>0.55972222222222223</v>
+        <v>0.5673611111111112</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4996,7 +4996,7 @@
       <c r="D15" s="17"/>
       <c r="E15" s="3">
         <f>E12+E13</f>
-        <v>0.58263888888888893</v>
+        <v>0.5902777777777779</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5008,7 +5008,7 @@
       <c r="D16" s="17"/>
       <c r="E16" s="3">
         <f>E15+TIME(0,(Données!E5*Données!F5),0)</f>
-        <v>0.63888888888888895</v>
+        <v>0.64652777777777792</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5020,7 +5020,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="4">
         <f>TIME(0,Données!G5,0)</f>
-        <v>6.9444444444444441E-3</v>
+        <v>9.7222222222222224E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5035,7 +5035,7 @@
       <c r="D18" s="15"/>
       <c r="E18" s="5">
         <f>E19-TIME(0,Données!D6,0)-TIME(0,Données!C6,0)</f>
-        <v>0.62291666666666667</v>
+        <v>0.63333333333333341</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5047,7 +5047,7 @@
       <c r="D19" s="17"/>
       <c r="E19" s="3">
         <f>E16+E17</f>
-        <v>0.64583333333333337</v>
+        <v>0.65625000000000011</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5059,7 +5059,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="6">
         <f>E19+TIME(0,(Données!E6*Données!F6),0)</f>
-        <v>0.70972222222222225</v>
+        <v>0.72013888888888899</v>
       </c>
     </row>
   </sheetData>
@@ -5091,6 +5091,6 @@
     <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>